<commit_message>
increased vols to 3 and 12
</commit_message>
<xml_diff>
--- a/source_plates/220208_source_plate.xlsx
+++ b/source_plates/220208_source_plate.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>A3,A4,A5,A6,A7,A8,A9,A10,A11,A12</t>
+          <t>A6,A7,A8,A9,A10,A11,A12</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -722,7 +722,7 @@
         <v>31</v>
       </c>
       <c r="F11" t="n">
-        <v>29</v>
+        <v>28.5</v>
       </c>
       <c r="G11" t="inlineStr"/>
     </row>
@@ -774,7 +774,7 @@
         <v>34</v>
       </c>
       <c r="F13" t="n">
-        <v>33</v>
+        <v>32.75</v>
       </c>
       <c r="G13" t="inlineStr"/>
     </row>
@@ -1280,7 +1280,7 @@
         <v>47.85</v>
       </c>
       <c r="F33" t="n">
-        <v>45.1</v>
+        <v>44.6</v>
       </c>
       <c r="G33" t="inlineStr"/>
     </row>
@@ -1332,7 +1332,7 @@
         <v>61.15</v>
       </c>
       <c r="F35" t="n">
-        <v>58.4</v>
+        <v>57.775</v>
       </c>
       <c r="G35" t="inlineStr"/>
     </row>

</xml_diff>